<commit_message>
The logic of comparison was created
</commit_message>
<xml_diff>
--- a/comentarios.xlsx
+++ b/comentarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arthur\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C0548B0-815A-4C1D-AB07-087297D6C6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCD69F3-BFEE-419A-B738-6C53F33210FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C2D7505A-E985-44B0-AB12-245393E9EBF8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>oi</t>
   </si>
@@ -53,12 +53,6 @@
     <t>saudades</t>
   </si>
   <si>
-    <t>digital</t>
-  </si>
-  <si>
-    <t>app</t>
-  </si>
-  <si>
     <t>pode falar</t>
   </si>
   <si>
@@ -75,6 +69,18 @@
   </si>
   <si>
     <t>unidade</t>
+  </si>
+  <si>
+    <t>alo digital no meio</t>
+  </si>
+  <si>
+    <t>app galera</t>
+  </si>
+  <si>
+    <t>saudades doi</t>
+  </si>
+  <si>
+    <t>digital galera</t>
   </si>
 </sst>
 </file>
@@ -130,8 +136,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7D57C609-6A0C-42DD-8FC6-68F105DCABF9}" name="Tabela2" displayName="Tabela2" ref="A1:B11" totalsRowShown="0">
-  <autoFilter ref="A1:B11" xr:uid="{7D57C609-6A0C-42DD-8FC6-68F105DCABF9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7D57C609-6A0C-42DD-8FC6-68F105DCABF9}" name="Tabela2" displayName="Tabela2" ref="A1:B13" totalsRowShown="0">
+  <autoFilter ref="A1:B13" xr:uid="{7D57C609-6A0C-42DD-8FC6-68F105DCABF9}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{F40B071F-D062-4C16-A207-D883C2EE98C2}" name="comentarios"/>
     <tableColumn id="2" xr3:uid="{02E6971F-D7ED-46B6-B2DA-208761C0A8D7}" name="unidade"/>
@@ -437,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC7C8A0D-D143-4E2A-B01A-3C0ABE4F9743}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,10 +457,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -484,33 +490,46 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>